<commit_message>
-- Feature  -- Affinity Operate procession
</commit_message>
<xml_diff>
--- a/data/亲和性试验配置.xlsx
+++ b/data/亲和性试验配置.xlsx
@@ -4,15 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18160" activeTab="5"/>
+    <workbookView windowHeight="18160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="communication" sheetId="2" r:id="rId1"/>
-    <sheet name="nodes" sheetId="3" r:id="rId2"/>
-    <sheet name="pods" sheetId="4" r:id="rId3"/>
-    <sheet name="d-agents" sheetId="5" r:id="rId4"/>
-    <sheet name="d-node_resource" sheetId="6" r:id="rId5"/>
-    <sheet name="d-communication" sheetId="7" r:id="rId6"/>
+    <sheet name="pods" sheetId="4" r:id="rId2"/>
+    <sheet name="nodes" sheetId="3" r:id="rId3"/>
+    <sheet name="d-node_resource" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>target</t>
   </si>
@@ -49,6 +47,12 @@
     <t>count</t>
   </si>
   <si>
+    <t>change_type</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
     <t>command_node-1</t>
   </si>
   <si>
@@ -94,27 +98,48 @@
     <t>aigc-4</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>aigc-5</t>
   </si>
   <si>
     <t>aigc-6</t>
   </si>
   <si>
+    <t>equipt-10</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>equipt-11</t>
+  </si>
+  <si>
+    <t>equipt-12</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
     <t>cpu</t>
   </si>
   <si>
+    <t>mem</t>
+  </si>
+  <si>
+    <t>gpu</t>
+  </si>
+  <si>
+    <t>disk</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
     <t>memory</t>
   </si>
   <si>
-    <t>gpu</t>
-  </si>
-  <si>
-    <t>disk</t>
-  </si>
-  <si>
     <t>net</t>
   </si>
   <si>
@@ -131,42 +156,6 @@
   </si>
   <si>
     <t>node-5</t>
-  </si>
-  <si>
-    <t>mem</t>
-  </si>
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>change_type</t>
-  </si>
-  <si>
-    <t>delay</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>equipt-10</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>equipt-11</t>
-  </si>
-  <si>
-    <t>equipt-12</t>
-  </si>
-  <si>
-    <t>platform-3</t>
-  </si>
-  <si>
-    <t>platform-10</t>
-  </si>
-  <si>
-    <t>platform-13</t>
   </si>
   <si>
     <t>cpu_used(cores)</t>
@@ -1346,15 +1335,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="30.0192307692308" customWidth="1"/>
+    <col min="2" max="2" width="26.0673076923077" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1370,13 +1364,19 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -1390,10 +1390,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
@@ -1424,10 +1424,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>6</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>6</v>
@@ -1458,10 +1458,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -1475,10 +1475,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
@@ -1492,10 +1492,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1543,10 +1543,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1560,10 +1560,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1575,12 +1575,12 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1591,13 +1591,19 @@
       <c r="E14" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1608,13 +1614,19 @@
       <c r="E15" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -1624,6 +1636,81 @@
       </c>
       <c r="E16" s="1">
         <v>6000</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>6000</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>6000</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>6000</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1633,6 +1720,430 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="43.9038461538462" customWidth="1"/>
+    <col min="7" max="7" width="15.6923076923077" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>2048</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>2048</v>
+      </c>
+      <c r="G17" t="str">
+        <f>+G16</f>
+        <v>-</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2048</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2048</v>
+      </c>
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>2048</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>2048</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F6"/>
@@ -1645,27 +2156,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -1685,7 +2196,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>32</v>
@@ -1705,7 +2216,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>32</v>
@@ -1725,7 +2236,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -1745,7 +2256,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>32</v>
@@ -1761,430 +2272,6 @@
       </c>
       <c r="F6">
         <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="1" width="43.9038461538462" customWidth="1"/>
-    <col min="7" max="7" width="15.6923076923077" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>3072</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>2048</v>
-      </c>
-      <c r="G16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>2048</v>
-      </c>
-      <c r="G17" t="str">
-        <f>+G16</f>
-        <v>-</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>2048</v>
-      </c>
-      <c r="G18" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>2048</v>
-      </c>
-      <c r="G19" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>2048</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>2048</v>
-      </c>
-      <c r="G21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2196,120 +2283,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="7"/>
-  <cols>
-    <col min="2" max="2" width="16.3365384615385" customWidth="1"/>
-    <col min="3" max="3" width="15.8557692307692" customWidth="1"/>
-    <col min="4" max="4" width="16.3461538461538" customWidth="1"/>
-    <col min="5" max="5" width="24.1923076923077" customWidth="1"/>
-    <col min="6" max="6" width="33.3269230769231" customWidth="1"/>
-    <col min="7" max="7" width="33.6442307692308" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1024</v>
-      </c>
-      <c r="E2">
-        <v>1024</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>1024</v>
-      </c>
-      <c r="E3">
-        <v>1024</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>2048</v>
-      </c>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
@@ -2325,30 +2301,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -2371,7 +2347,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -2394,7 +2370,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -2417,7 +2393,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -2440,7 +2416,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -2459,539 +2435,6 @@
       </c>
       <c r="G6">
         <v>8000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AX16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
-  <cols>
-    <col min="46" max="46" width="35.5673076923077" customWidth="1"/>
-    <col min="47" max="47" width="49.5192307692308" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:50">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>6000</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AV2">
-        <v>2</v>
-      </c>
-      <c r="AW2">
-        <v>6</v>
-      </c>
-      <c r="AX2">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>6000</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AV3">
-        <v>5</v>
-      </c>
-      <c r="AW3">
-        <v>2</v>
-      </c>
-      <c r="AX3">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>6000</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV4">
-        <v>6</v>
-      </c>
-      <c r="AW4">
-        <v>4</v>
-      </c>
-      <c r="AX4">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>6000</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV5">
-        <v>6</v>
-      </c>
-      <c r="AW5">
-        <v>1</v>
-      </c>
-      <c r="AX5">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>6000</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV6">
-        <v>6</v>
-      </c>
-      <c r="AW6">
-        <v>1</v>
-      </c>
-      <c r="AX6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>6000</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV7">
-        <v>6</v>
-      </c>
-      <c r="AW7">
-        <v>2</v>
-      </c>
-      <c r="AX7">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>6000</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV8">
-        <v>6</v>
-      </c>
-      <c r="AW8">
-        <v>1</v>
-      </c>
-      <c r="AX8">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:50">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>6000</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV9">
-        <v>8</v>
-      </c>
-      <c r="AW9">
-        <v>4</v>
-      </c>
-      <c r="AX9">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>6000</v>
-      </c>
-      <c r="AT10" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AV10">
-        <v>7</v>
-      </c>
-      <c r="AW10">
-        <v>1</v>
-      </c>
-      <c r="AX10">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>6000</v>
-      </c>
-      <c r="AT11" t="s">
-        <v>9</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV11">
-        <v>2</v>
-      </c>
-      <c r="AW11">
-        <v>9</v>
-      </c>
-      <c r="AX11">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:50">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>6000</v>
-      </c>
-      <c r="AT12" t="s">
-        <v>11</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>17</v>
-      </c>
-      <c r="AV12">
-        <v>1</v>
-      </c>
-      <c r="AW12">
-        <v>6</v>
-      </c>
-      <c r="AX12">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:50">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>6000</v>
-      </c>
-      <c r="AT13" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>18</v>
-      </c>
-      <c r="AV13">
-        <v>2</v>
-      </c>
-      <c r="AW13">
-        <v>8</v>
-      </c>
-      <c r="AX13">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:50">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>9</v>
-      </c>
-      <c r="E14">
-        <v>6000</v>
-      </c>
-      <c r="AT14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>19</v>
-      </c>
-      <c r="AV14">
-        <v>2</v>
-      </c>
-      <c r="AW14">
-        <v>9</v>
-      </c>
-      <c r="AX14">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:50">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>6000</v>
-      </c>
-      <c r="AT15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV15">
-        <v>1</v>
-      </c>
-      <c r="AW15">
-        <v>9</v>
-      </c>
-      <c r="AX15">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:50">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>9</v>
-      </c>
-      <c r="E16">
-        <v>6000</v>
-      </c>
-      <c r="AT16" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU16" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV16">
-        <v>2</v>
-      </c>
-      <c r="AW16">
-        <v>9</v>
-      </c>
-      <c r="AX16">
-        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>